<commit_message>
Modify train.py to read data.
</commit_message>
<xml_diff>
--- a/cost.xlsx
+++ b/cost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sentry\Documents\Stanford.9\CS 230\image-outpainting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3141F822-A016-4921-BA15-F621C6315262}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3EBD6821-272A-44D1-A852-CD27F19FE8C2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" xr2:uid="{C5E310BA-986E-4C9E-A066-4D9D1071D560}"/>
   </bookViews>
@@ -451,7 +451,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,11 +552,11 @@
         <v>22.6</v>
       </c>
       <c r="M2" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="N2">
         <f>D2*L2*2/M2/1000</f>
-        <v>102.83</v>
+        <v>51.414999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Modify sync.sh to use rsync, to only copy new files.
</commit_message>
<xml_diff>
--- a/cost.xlsx
+++ b/cost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sentry\Documents\Stanford.9\CS 230\image-outpainting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3EBD6821-272A-44D1-A852-CD27F19FE8C2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CB101D68-2AC4-4E04-9563-5395058331F9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" xr2:uid="{C5E310BA-986E-4C9E-A066-4D9D1071D560}"/>
   </bookViews>
@@ -63,10 +63,10 @@
     <t>img_size (KB)</t>
   </si>
   <si>
-    <t>SAVE_INTV</t>
-  </si>
-  <si>
     <t>img_size (MB)</t>
+  </si>
+  <si>
+    <t>INTV_PRINT</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,10 +501,10 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -549,14 +549,14 @@
         <v>182000</v>
       </c>
       <c r="L2">
-        <v>22.6</v>
+        <v>30</v>
       </c>
       <c r="M2" s="1">
         <v>200</v>
       </c>
       <c r="N2">
-        <f>D2*L2*2/M2/1000</f>
-        <v>51.414999999999999</v>
+        <f>D2*L2*11/M2/1000</f>
+        <v>375.375</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add model5 for local discriminator, and train_ld.py.
</commit_message>
<xml_diff>
--- a/cost.xlsx
+++ b/cost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sentry\Documents\Stanford.9\CS 230\image-outpainting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CB101D68-2AC4-4E04-9563-5395058331F9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C4B8076F-CAEE-4994-88CE-57AE680A6EBD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" xr2:uid="{C5E310BA-986E-4C9E-A066-4D9D1071D560}"/>
   </bookViews>
@@ -451,7 +451,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,13 +561,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>30</v>
+        <v>3000</v>
       </c>
       <c r="D3">
         <f>C3*A3/B3</f>
@@ -578,15 +578,15 @@
       </c>
       <c r="F3">
         <f>(16/B3) *E3</f>
-        <v>3.2</v>
+        <v>32</v>
       </c>
       <c r="G3">
         <f>D3/F3</f>
-        <v>937.5</v>
+        <v>93.75</v>
       </c>
       <c r="H3">
         <f>G3/3600</f>
-        <v>0.26041666666666669</v>
+        <v>2.6041666666666668E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>